<commit_message>
chore: update config and sync Excel file to repository
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="11920"/>
+    <workbookView windowWidth="30740" windowHeight="16340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -96,7 +96,7 @@
     <t>https://ferrumdecorstudio.shop/products/pure-brass-personalized-letter-box-modern-wall-mount-brass-mailbox-unique-personalized-post-box-copy</t>
   </si>
   <si>
-    <t>From $949.00 USD✏️</t>
+    <t>$949.00 USD</t>
   </si>
   <si>
     <t>https://ferrumdecorstudio.shop/cdn/shop/files/8d31766a22fd145253229f80d9d90532.jpg?v=1736934924</t>
@@ -159,13 +159,13 @@
     <t>https://ferrumdecorstudio.shop/products/pure-brass-personalized-mailbox-copy</t>
   </si>
   <si>
-    <t>From $395.00 USD✏️</t>
-  </si>
-  <si>
     <t>https://ferrumdecorstudio.shop/cdn/shop/files/dd.jpg?v=1736779301</t>
   </si>
   <si>
     <t>https://ferrumdecorstudio.shop/products/bespoke-custom-built-wall-mount-cor-ten-steel-mailbox-copy</t>
+  </si>
+  <si>
+    <t>$949.00 USD✏️</t>
   </si>
   <si>
     <t>https://ferrumdecorstudio.shop/cdn/shop/files/hhh.jpg?v=1736778850</t>
@@ -1338,8 +1338,8 @@
   <sheetPr/>
   <dimension ref="A1:A168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="A144" sqref="A144"/>
+    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
@@ -2092,7 +2092,7 @@
     </row>
     <row r="149" spans="1:1">
       <c r="A149" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="150" spans="1:1">
@@ -2112,7 +2112,7 @@
     </row>
     <row r="153" spans="1:1">
       <c r="A153" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="154" spans="1:1">
@@ -2127,7 +2127,7 @@
     </row>
     <row r="156" spans="1:1">
       <c r="A156" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="157" spans="1:1">
@@ -2137,7 +2137,7 @@
     </row>
     <row r="158" spans="1:1">
       <c r="A158" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
     </row>
     <row r="159" spans="1:1">

</xml_diff>